<commit_message>
feat(specialties): :sparkles: config specialties excel report
</commit_message>
<xml_diff>
--- a/public/templates/professionalContract.xlsx
+++ b/public/templates/professionalContract.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\09.- PROCESOS DE SELECCION\PROCESOS 2023\27.- CHECCA IES INTEQ CANCHA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gpro1\MyFiles\QuisVar\quisvar_proyect_ft\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C946DD1-47F1-4C18-A2DC-1DE0E9B27021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C3C742-B965-46BB-BE2B-064849C47AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{67D68625-E83D-4895-B9F2-E4D05BDD5F55}"/>
   </bookViews>
@@ -17,7 +17,8 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$D$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$E$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Hoja2!$A$1:$G$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,13 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
-  <si>
-    <t xml:space="preserve">JEFE DE PROYECTO </t>
-  </si>
-  <si>
-    <t>CIP</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t xml:space="preserve">NOMBRES Y APELLIDOS </t>
   </si>
@@ -52,21 +47,6 @@
     <t>CARGO</t>
   </si>
   <si>
-    <t xml:space="preserve">ESPECIALISTA EN ESTRUCTURAS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESPECIALISTA EN ARQUITECTURA </t>
-  </si>
-  <si>
-    <t>ESPECIALISTA EN ELCTRICAS</t>
-  </si>
-  <si>
-    <t>ESPECIALISTA EN SANITARIAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESPECIALISTA EN COSTOS Y PRESUPUESTOS </t>
-  </si>
-  <si>
     <t xml:space="preserve">REPRESENTANTE </t>
   </si>
   <si>
@@ -85,27 +65,6 @@
     <t>“MEJORAMIENTO DEL SERVICIO DE EDUCACIÓN SECUNDARIA EN I.E. INTEQ KANCHAN DE CENTRO POBLADO HANANSAYA DISTRITO DE CHECCA DE LA PROVINCIA DE CANAS DEL DEPARTAMENTO DE CUSCO”</t>
   </si>
   <si>
-    <t>CLEVER LARICO CONDORI</t>
-  </si>
-  <si>
-    <t>RONAL NILTON CHAMBI MAMANI</t>
-  </si>
-  <si>
-    <t>LUDWING LI GOMEZ BAILON</t>
-  </si>
-  <si>
-    <t>CAP 16053</t>
-  </si>
-  <si>
-    <t>AQUILES MACHACA HUANCA</t>
-  </si>
-  <si>
-    <t>RODRIGUEZ TRUJILLO LESLY DIOSHELYN NIMYA</t>
-  </si>
-  <si>
-    <t>ELISMAN LOPEZ AMPUERO</t>
-  </si>
-  <si>
     <t>ROSENDO CONDORI QUISPE</t>
   </si>
   <si>
@@ -122,13 +81,16 @@
   </si>
   <si>
     <t>TOTAL PAGO</t>
+  </si>
+  <si>
+    <t>COLEGIATURA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +140,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bahnschrift SemiBold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -266,24 +243,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -293,7 +269,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -305,7 +281,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -325,70 +301,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2160134</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>76541</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>489676</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>77221</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{713767B5-C746-4AC2-9723-9B2BEB455CD7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="21257" t="18099" r="20359" b="26697"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2398259" y="3087121"/>
-          <a:ext cx="897890" cy="561975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -426,7 +342,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -532,7 +448,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -674,7 +590,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -682,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D09FE9-7A07-4C01-B301-65C7A2D6F3B6}">
-  <dimension ref="B2:D21"/>
+  <dimension ref="B2:D24"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="112" zoomScaleNormal="100" zoomScaleSheetLayoutView="112" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C13"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScale="112" zoomScaleNormal="100" zoomScaleSheetLayoutView="112" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,158 +609,112 @@
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" customWidth="1"/>
     <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+      <c r="B3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="2:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
     </row>
     <row r="6" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="B6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2">
-        <v>194067</v>
-      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2">
-        <v>190511</v>
-      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2">
-        <v>103260</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="2">
-        <v>221911</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="2">
-        <v>209087</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -852,21 +722,20 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="91" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161C8D83-2734-414A-A71F-C0144116B57A}">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:F11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,150 +745,76 @@
     <col min="3" max="3" width="38.140625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="2:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="B3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="B4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="8">
-        <v>500</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="8">
-        <v>300</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="8">
-        <v>300</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="8">
-        <v>300</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="8">
-        <v>300</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="8">
-        <v>300</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="10">
-        <f>SUM(D6:D11)</f>
-        <v>2000</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="6" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="94" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>